<commit_message>
removed return that stopped code after 1 mesh
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774D1DDC-932A-4094-B597-F98A06F5BF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA0485-BEC4-4680-8900-6F124E1F8961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20865" yWindow="2835" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ready to run landmarking on untextured meshes
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA0485-BEC4-4680-8900-6F124E1F8961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E133E00-F346-43AD-BC33-0BEE6FA3F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20865" yWindow="2835" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>data_type</t>
   </si>
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +751,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
executed hsa on textured meshes
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E133E00-F346-43AD-BC33-0BEE6FA3F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EF6DF8-28EB-4FFA-819D-0A7EFCD8920F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>data_type</t>
   </si>
@@ -451,31 +451,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -522,7 +522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -792,6 +792,50 @@
         <v>0</v>
       </c>
       <c r="O7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made hsa ready to run in cluster
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EF6DF8-28EB-4FFA-819D-0A7EFCD8920F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2089B9E-AE27-4634-8237-3E34280C8FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>data_type</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>C:\Users\franz\Documents\work\projects\arp\data\synthetic_data\synthetic_data_original_textured_unclipped_vtp_paraview</t>
+  </si>
+  <si>
+    <t>/data/scratch/r092382/synthetic_data/synthetic_data_original_textured_unclipped_vtp_paraview_sample</t>
   </si>
 </sst>
 </file>
@@ -451,31 +454,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.33203125" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -522,7 +525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -569,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -616,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -707,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -795,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -836,6 +839,50 @@
         <v>1</v>
       </c>
       <c r="O8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran HSA with 27 landmarks
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BE0DC-8EF5-4D1E-A10B-4AD54F3DE83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8515F446-38AE-40D0-9CC0-BC563FC5D9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>data_type</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>/data/scratch/r092382/synthetic_data/synthetic_data_original_textured_unclipped_vtp_paraview_sample</t>
+  </si>
+  <si>
+    <t>{"TRAGION_RIGHT": "4869", "SELLION": "3410", "TRAGION_LEFT": "2431", "EURYON_RIGHT": "138", "EURYON_LEFT": "5752", "FRONTOTEMPORALE_RIGHT": "7395", "FRONTOTEMPORALE_LEFT": "4503", "VERTEX": "8614", "NASION": "9396", "GLABELLA": "4328", "OPISTHOCRANION": "8232", "GNATHION": "6703", "STOMION": "3171", "ZYGION_RIGHT": "5549", "ZYGION_LEFT": "2764", "GONION_RIGHT": "10595", "GONION_LEFT": "6576", "SUBNASALE": "6274", "ENDOCANTHION_RIGHT": "678", "ENDOCANTHION_LEFT": "2102", "EXOCANTHION_RIGHT": "4197", "EXOCANTHION_LEFT": "2063", "ALAR_RIGHT": "1706", "ALAR_LEFT": "281", "NASALE_TIP": "6280", "SUBLABIALE": "9124", "UPPER_LIP": "6083"}</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\synthetic_data\synthetic_data_original_untextured_unclipped_vtp_27v3_comp</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023</t>
   </si>
 </sst>
 </file>
@@ -454,31 +466,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -525,7 +537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -572,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -619,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -666,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -710,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -754,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -798,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -842,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -884,6 +896,120 @@
       </c>
       <c r="O9" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began hsa exec for patient data
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8515F446-38AE-40D0-9CC0-BC563FC5D9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADC8E60-66D6-4C27-B225-0256E0A864E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
   <si>
     <t>data_type</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023</t>
+  </si>
+  <si>
+    <t>_neck_clipped.obj</t>
   </si>
 </sst>
 </file>
@@ -468,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,7 +1009,7 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="K12" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
prepared hsa calculator for patient data
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADC8E60-66D6-4C27-B225-0256E0A864E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BADBC4-CDC3-42D9-9C73-AECDAEE17781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>data_type</t>
   </si>
@@ -127,6 +138,15 @@
   </si>
   <si>
     <t>_neck_clipped.obj</t>
+  </si>
+  <si>
+    <t>.obj</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023\sagittal_patient_data_sept2023_age_sex_data.xlsx</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -469,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,10 +1029,39 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12" t="s">
         <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get patient age and sex
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BADBC4-CDC3-42D9-9C73-AECDAEE17781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D7891-2CCF-41FB-AF95-29D3928E68A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="-15480" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,10 +143,10 @@
     <t>.obj</t>
   </si>
   <si>
-    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023\sagittal_patient_data_sept2023_age_sex_data.xlsx</t>
-  </si>
-  <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\patient_information.xlsx</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,10 +1032,10 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
completed hsa executor for patient data
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2D7891-2CCF-41FB-AF95-29D3928E68A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33565C8A-4E7E-478C-93D7-F72A5DF037A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="-15480" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>data_type</t>
   </si>
@@ -137,16 +137,19 @@
     <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023</t>
   </si>
   <si>
-    <t>_neck_clipped.obj</t>
-  </si>
-  <si>
-    <t>.obj</t>
-  </si>
-  <si>
     <t>_</t>
   </si>
   <si>
     <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\patient_information.xlsx</t>
+  </si>
+  <si>
+    <t>sagittal</t>
+  </si>
+  <si>
+    <t>_neck_cropped.obj</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sample_data</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,6 +1025,9 @@
       <c r="B12" t="s">
         <v>31</v>
       </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
@@ -1029,13 +1035,13 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
         <v>34</v>
       </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1047,21 +1053,63 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="M12" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
       <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
         <v>33</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cloned repo into cpu cluster
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9FDA8-A696-45DF-B484-9A041EFE934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AC0AFD-373C-4863-825E-FD4A9CDCDFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
   <si>
     <t>data_type</t>
   </si>
@@ -137,19 +137,25 @@
     <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sagittal_patient_data_sept2023</t>
   </si>
   <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\patient_information.xlsx</t>
+  </si>
+  <si>
+    <t>sagittal</t>
+  </si>
+  <si>
+    <t>_neck_cropped.obj</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sample_data</t>
+  </si>
+  <si>
     <t>_</t>
   </si>
   <si>
-    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\patient_information.xlsx</t>
-  </si>
-  <si>
-    <t>sagittal</t>
-  </si>
-  <si>
-    <t>_neck_cropped.obj</t>
-  </si>
-  <si>
-    <t>C:\Users\franz\Documents\work\projects\arp\data\patient_data\sample_data</t>
+    <t>export_vtp_mesh</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,11 +518,12 @@
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -554,16 +561,19 @@
         <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -601,7 +611,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="2" t="b">
         <v>1</v>
@@ -609,8 +619,11 @@
       <c r="O2" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -647,17 +660,20 @@
       <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="b">
-        <v>1</v>
+      <c r="M3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -694,8 +710,8 @@
       <c r="L4" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="b">
-        <v>1</v>
+      <c r="M4" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
@@ -703,8 +719,11 @@
       <c r="O4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -738,8 +757,8 @@
       <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="M5" t="b">
-        <v>1</v>
+      <c r="M5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N5" t="b">
         <v>1</v>
@@ -747,8 +766,11 @@
       <c r="O5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -782,17 +804,20 @@
       <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="M6" t="b">
-        <v>1</v>
+      <c r="M6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -826,17 +851,20 @@
       <c r="K7" t="s">
         <v>26</v>
       </c>
-      <c r="M7" t="b">
-        <v>1</v>
+      <c r="M7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -870,17 +898,20 @@
       <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="M8" t="b">
+      <c r="M8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -914,17 +945,20 @@
       <c r="K9" t="s">
         <v>26</v>
       </c>
-      <c r="M9" t="b">
+      <c r="M9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -961,8 +995,8 @@
       <c r="L10" t="s">
         <v>24</v>
       </c>
-      <c r="M10" t="b">
-        <v>1</v>
+      <c r="M10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N10" t="b">
         <v>1</v>
@@ -970,8 +1004,11 @@
       <c r="O10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1008,8 +1045,8 @@
       <c r="L11" t="s">
         <v>29</v>
       </c>
-      <c r="M11" t="b">
-        <v>1</v>
+      <c r="M11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N11" t="b">
         <v>1</v>
@@ -1017,8 +1054,11 @@
       <c r="O11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1026,7 +1066,7 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1035,13 +1075,13 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1050,22 +1090,25 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="L12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" t="b">
+        <v>37</v>
+      </c>
+      <c r="M12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="N12" t="b">
         <v>0</v>
       </c>
       <c r="O12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1073,22 +1116,22 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -1100,15 +1143,18 @@
         <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M13" t="b">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="M13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="N13" t="b">
         <v>1</v>
       </c>
       <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
specified landmarks naming and which subtypes folders to run
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AC0AFD-373C-4863-825E-FD4A9CDCDFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA351E-6688-46B6-94CA-C3FDAC8701CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="43">
   <si>
     <t>data_type</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>included_subtypes</t>
+  </si>
+  <si>
+    <t>metopic, sagittal</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -187,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,14 +219,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,19 +532,20 @@
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="125.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -540,40 +562,43 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -589,32 +614,32 @@
       <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>200</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="N2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2" t="b">
         <v>1</v>
@@ -622,8 +647,11 @@
       <c r="P2" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -639,41 +667,44 @@
       <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>200</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <v>1</v>
+      <c r="N3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -690,31 +721,31 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>200</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
+      <c r="N4" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
@@ -722,8 +753,11 @@
       <c r="P4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -737,31 +771,31 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>200</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
+      <c r="N5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
@@ -769,8 +803,11 @@
       <c r="P5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -787,37 +824,40 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>200</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
+      <c r="N6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -834,37 +874,40 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>200</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" t="b">
-        <v>1</v>
+      <c r="N7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -881,37 +924,40 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>200</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" t="b">
+      <c r="N8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="O8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -928,37 +974,40 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>200</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
+      <c r="N9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="O9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -975,31 +1024,31 @@
         <v>30</v>
       </c>
       <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>200</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <v>1</v>
+      <c r="N10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O10" t="b">
         <v>1</v>
@@ -1007,8 +1056,11 @@
       <c r="P10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1025,31 +1077,31 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>200</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <v>1</v>
+      <c r="N11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O11" t="b">
         <v>1</v>
@@ -1057,8 +1109,11 @@
       <c r="P11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1075,40 +1130,43 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
         <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>39</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
+      <c r="N12" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="O12" t="b">
         <v>0</v>
       </c>
       <c r="P12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1125,36 +1183,92 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
         <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
       </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>1</v>
+      <c r="N13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="O13" t="b">
         <v>1</v>
       </c>
       <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>200</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hsa ready for synthetic ori
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA351E-6688-46B6-94CA-C3FDAC8701CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B44FA1-968D-40BD-9039-451E80FF8866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,13 +521,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
hsa exports with landmarks number
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B44FA1-968D-40BD-9039-451E80FF8866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E3B3D3-05D2-4C0B-B5F0-00F55299701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,10 +161,10 @@
     <t>included_subtypes</t>
   </si>
   <si>
+    <t>all</t>
+  </si>
+  <si>
     <t>metopic, sagittal</t>
-  </si>
-  <si>
-    <t>all</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>17</v>
@@ -668,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
@@ -721,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -824,7 +824,7 @@
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
@@ -874,7 +874,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
@@ -924,7 +924,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -974,7 +974,7 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -1024,7 +1024,7 @@
         <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -1077,7 +1077,7 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
@@ -1130,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
         <v>35</v>
@@ -1183,7 +1183,7 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
         <v>35</v>
@@ -1236,7 +1236,7 @@
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
created a visualisation use case
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F9C59C-1804-40CA-867A-400BF3995140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22868477-D9D3-4391-ABBC-035EF764640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,10 +164,10 @@
     <t>all</t>
   </si>
   <si>
-    <t>metopic, sagittal</t>
-  </si>
-  <si>
     <t>{"TRAGION_RIGHT": "4869", "SELLION": "3410", "TRAGION_LEFT": "2431", "EURYON_RIGHT": "10278", "EURYON_LEFT": "8793", "FRONTOTEMPORALE_RIGHT": "7395", "FRONTOTEMPORALE_LEFT": "4503", "VERTEX": "8614", "NASION": "9396", "GLABELLA": "4328", "OPISTHOCRANION": "5335", "GNATHION": "6703", "STOMION": "3171", "ZYGION_RIGHT": "5549", "ZYGION_LEFT": "2764", "GONION_RIGHT": "10595", "GONION_LEFT": "6576", "SUBNASALE": "6274", "ENDOCANTHION_RIGHT": "678", "ENDOCANTHION_LEFT": "2102", "EXOCANTHION_RIGHT": "4197", "EXOCANTHION_LEFT": "2063", "ALAR_RIGHT": "1706", "ALAR_LEFT": "281", "NASALE_TIP": "6280", "SUBLABIALE": "9124", "UPPER_LIP": "6083"}</t>
+  </si>
+  <si>
+    <t>coronal</t>
   </si>
 </sst>
 </file>
@@ -524,31 +524,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.33203125" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -601,7 +601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -810,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -960,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
@@ -1260,7 +1260,7 @@
         <v>25</v>
       </c>
       <c r="M14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N14" s="3" t="b">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="P14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
set hsa output to within repo
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22868477-D9D3-4391-ABBC-035EF764640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD20502-0994-4AD6-B4EC-76FB3828088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="46">
   <si>
     <t>data_type</t>
   </si>
@@ -167,7 +167,13 @@
     <t>{"TRAGION_RIGHT": "4869", "SELLION": "3410", "TRAGION_LEFT": "2431", "EURYON_RIGHT": "10278", "EURYON_LEFT": "8793", "FRONTOTEMPORALE_RIGHT": "7395", "FRONTOTEMPORALE_LEFT": "4503", "VERTEX": "8614", "NASION": "9396", "GLABELLA": "4328", "OPISTHOCRANION": "5335", "GNATHION": "6703", "STOMION": "3171", "ZYGION_RIGHT": "5549", "ZYGION_LEFT": "2764", "GONION_RIGHT": "10595", "GONION_LEFT": "6576", "SUBNASALE": "6274", "ENDOCANTHION_RIGHT": "678", "ENDOCANTHION_LEFT": "2102", "EXOCANTHION_RIGHT": "4197", "EXOCANTHION_LEFT": "2063", "ALAR_RIGHT": "1706", "ALAR_LEFT": "281", "NASALE_TIP": "6280", "SUBLABIALE": "9124", "UPPER_LIP": "6083"}</t>
   </si>
   <si>
-    <t>coronal</t>
+    <t>metopic, sagittal</t>
+  </si>
+  <si>
+    <t>metopic</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\synthetic_data\synthetic_data_original_textured_unclipped_vtp_expanded_to_pat_sag_1716156_pre</t>
   </si>
 </sst>
 </file>
@@ -522,33 +528,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="125.28515625" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="66.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -601,7 +607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -654,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -707,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -760,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -810,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -860,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -960,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
@@ -1266,12 +1272,65 @@
         <v>0</v>
       </c>
       <c r="O14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>235</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
got latest upstream code and separated hsa version call
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD20502-0994-4AD6-B4EC-76FB3828088E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0ACE38-7D09-43AA-928D-4449CD31D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
   <si>
     <t>data_type</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>C:\Users\franz\Documents\work\projects\arp\data\synthetic_data\synthetic_data_original_textured_unclipped_vtp_expanded_to_pat_sag_1716156_pre</t>
+  </si>
+  <si>
+    <t>hsa_model</t>
+  </si>
+  <si>
+    <t>C:\Users\franz\Documents\work\projects\arp\data\synthetic_data\synthetic_data_original_textured_metopic_61_vtp</t>
   </si>
 </sst>
 </file>
@@ -528,130 +534,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="125.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>200</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="2" t="b">
-        <v>0</v>
-      </c>
       <c r="O2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="2" t="b">
         <v>1</v>
@@ -659,105 +667,105 @@
       <c r="Q2" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>200</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
-        <v>1</v>
+      <c r="O3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>200</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>6</v>
       </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" t="b">
-        <v>1</v>
+      <c r="O4" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P4" t="b">
         <v>1</v>
@@ -765,49 +773,49 @@
       <c r="Q4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
       <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>41</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>200</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>25</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
-        <v>1</v>
+      <c r="O5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P5" t="b">
         <v>1</v>
@@ -815,252 +823,252 @@
       <c r="Q5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
       <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>200</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" t="b">
-        <v>1</v>
+      <c r="O6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
       <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>200</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>6</v>
       </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
-        <v>1</v>
+      <c r="O7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
       <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>200</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
         <v>26</v>
       </c>
-      <c r="N8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" t="b">
+      <c r="O8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
       <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>200</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>6</v>
       </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
+      <c r="O9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="P9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
       <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>200</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>6</v>
       </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>25</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <v>1</v>
+      <c r="O10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P10" t="b">
         <v>1</v>
@@ -1068,52 +1076,52 @@
       <c r="Q10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
       <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>18</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>200</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>6</v>
       </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>25</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" t="b">
-        <v>1</v>
+      <c r="O11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P11" t="b">
         <v>1</v>
@@ -1121,105 +1129,105 @@
       <c r="Q11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
       </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>39</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="b">
-        <v>0</v>
+      <c r="O12" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
       </c>
       <c r="Q12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>36</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>41</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>33</v>
       </c>
       <c r="I13" t="s">
         <v>33</v>
       </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>26</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>37</v>
       </c>
-      <c r="N13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O13" t="b">
-        <v>1</v>
+      <c r="O13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="P13" t="b">
         <v>1</v>
@@ -1227,110 +1235,119 @@
       <c r="Q13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>1</v>
+      <c r="B14">
+        <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
+      <c r="E14" t="b">
+        <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>200</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>6</v>
       </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
         <v>25</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O14" t="b">
+      <c r="O14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="P14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>43</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>235</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>6</v>
       </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
         <v>25</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>42</v>
       </c>
-      <c r="N15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="O15" t="b">
+      <c r="O15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="P15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
can run HSA v1 and v2
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
+++ b/franz_hsa/landmark_pred_n_hsa_calc/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_pred_n_hsa_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0ACE38-7D09-43AA-928D-4449CD31D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B0AEF6-5062-4C7F-9594-1B8819554829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1244,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>

</xml_diff>